<commit_message>
New objective for run, updates for geospatial optimisation
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Tanzania/optimisationBudgets.xlsx
+++ b/input_spreadsheets/Tanzania/optimisationBudgets.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/input_spreadsheets/Tanzania/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25DA5E0F-2C1B-D846-9CE6-54D050A175FD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{618988BE-F284-CD40-B4BB-F8A6D89F54A8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-21140" windowWidth="38400" windowHeight="21140" activeTab="1" xr2:uid="{6937E72E-728A-D145-8CDA-D71DF27F887B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19200" windowHeight="15540" xr2:uid="{6937E72E-728A-D145-8CDA-D71DF27F887B}"/>
   </bookViews>
   <sheets>
     <sheet name="Current expenditure" sheetId="1" r:id="rId1"/>
     <sheet name="Optimal funding scenario" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -155,7 +155,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
   <si>
     <t>Region</t>
   </si>
@@ -352,6 +352,21 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>Kaskazini Unguja</t>
+  </si>
+  <si>
+    <t>Kaskazini Pemba</t>
+  </si>
+  <si>
+    <t>Kusini Pemba</t>
+  </si>
+  <si>
+    <t>Kusini Unguja</t>
+  </si>
+  <si>
+    <t>Mjini Magharibi</t>
   </si>
 </sst>
 </file>
@@ -800,15 +815,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{875686D2-62DB-5148-AE87-D8FE690481A1}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" customWidth="1"/>
     <col min="2" max="2" width="17.1640625" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
   </cols>
@@ -850,142 +865,180 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5">
-        <v>65831.185454545455</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="B5" s="5"/>
       <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="5">
-        <v>203617.48545454544</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="B6" s="5"/>
       <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B7" s="5">
-        <v>204623.54545454544</v>
+        <v>65831.185454545455</v>
       </c>
       <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B8" s="5">
-        <v>811987.85090909095</v>
+        <v>203617.48545454544</v>
       </c>
       <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="5">
-        <v>291253.25028181821</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="B9" s="5"/>
       <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="5">
-        <v>3456219.3768181819</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="B10" s="5"/>
       <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B11" s="5">
-        <v>233815.43454545454</v>
+        <v>204623.54545454544</v>
       </c>
       <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B12" s="5">
-        <v>306057.97045454546</v>
+        <v>811987.85090909095</v>
       </c>
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B13" s="5">
-        <v>143226.44545454546</v>
+        <v>291253.25028181821</v>
       </c>
       <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="5">
-        <v>682360.4718181818</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="B14" s="5"/>
       <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B15" s="5">
-        <v>641061.65625</v>
+        <v>3456219.3768181819</v>
       </c>
       <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B16" s="5">
-        <v>451140.74136363639</v>
+        <v>233815.43454545454</v>
       </c>
       <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B17" s="5">
-        <v>328555.68181818182</v>
+        <v>306057.97045454546</v>
       </c>
       <c r="E17" s="3"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="5">
+        <v>143226.44545454546</v>
+      </c>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="5">
+        <v>682360.4718181818</v>
+      </c>
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="5">
+        <v>641061.65625</v>
+      </c>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="5">
+        <v>451140.74136363639</v>
+      </c>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="5">
+        <v>328555.68181818182</v>
+      </c>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B23" s="5">
         <v>378379.0459090909</v>
       </c>
-      <c r="E18" s="3"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="7">
-        <f>SUM(B2:B18)</f>
+      <c r="B24" s="7">
+        <f>SUM(B2:B23)</f>
         <v>9891483.4535681829</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B20" s="2"/>
-      <c r="E20" s="3"/>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B25" s="2"/>
+      <c r="E25" s="3"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B28" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -998,8 +1051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60C6C199-5511-6948-BFE1-269E2A0DC50C}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1041,9 +1094,7 @@
       <c r="D2" s="11">
         <v>0</v>
       </c>
-      <c r="E2" s="12" t="s">
-        <v>20</v>
-      </c>
+      <c r="E2" s="12"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
@@ -1058,9 +1109,7 @@
       <c r="D3" s="11">
         <v>0</v>
       </c>
-      <c r="E3" s="12" t="s">
-        <v>20</v>
-      </c>
+      <c r="E3" s="12"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
@@ -1094,9 +1143,7 @@
         <f>(20+30+45+45+35+22)/6 * 1000000</f>
         <v>32833333.333333336</v>
       </c>
-      <c r="E5" s="12" t="s">
-        <v>20</v>
-      </c>
+      <c r="E5" s="12"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">

</xml_diff>

<commit_message>
Optimising for healthy children, new version of ASD
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Tanzania/optimisationBudgets.xlsx
+++ b/input_spreadsheets/Tanzania/optimisationBudgets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/input_spreadsheets/Tanzania/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{A4A5EDA3-E15F-FE44-8370-F9C7075C08AB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{26977A23-D745-6343-868B-1A9CE42FD9B0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19200" windowHeight="15540" xr2:uid="{6937E72E-728A-D145-8CDA-D71DF27F887B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19200" windowHeight="15540" activeTab="1" xr2:uid="{6937E72E-728A-D145-8CDA-D71DF27F887B}"/>
   </bookViews>
   <sheets>
     <sheet name="Current expenditure" sheetId="1" r:id="rId1"/>
@@ -84,6 +84,39 @@
     <author>Sam</author>
   </authors>
   <commentList>
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{5DD8B547-D8D5-7549-A948-7A084F42ED59}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Average annual spending 2019-2024 from Yi-Kyoung</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="D4" authorId="0" shapeId="0" xr:uid="{3F519331-3FEE-8242-AC5A-60B03343E38E}">
       <text>
         <r>
@@ -824,7 +857,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{875686D2-62DB-5148-AE87-D8FE690481A1}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+    <sheetView zoomScale="125" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -1068,8 +1101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60C6C199-5511-6948-BFE1-269E2A0DC50C}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1106,12 +1139,15 @@
         <v>27</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" s="11">
-        <v>0</v>
-      </c>
-      <c r="E2" s="12"/>
+        <v>28</v>
+      </c>
+      <c r="D2" s="13">
+        <f>(20+30+45+45+35+22)/6 * 1000000</f>
+        <v>32833333.333333336</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
@@ -1142,9 +1178,7 @@
         <f>(20+30+45+45+35+22)/6 * 1000000</f>
         <v>32833333.333333336</v>
       </c>
-      <c r="E4" s="12" t="s">
-        <v>20</v>
-      </c>
+      <c r="E4" s="12"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">

</xml_diff>

<commit_message>
Added new param for calibration
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Tanzania/optimisationBudgets.xlsx
+++ b/input_spreadsheets/Tanzania/optimisationBudgets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/input_spreadsheets/Tanzania/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{B5EC0ABE-31C8-4747-BFA1-FA0FEA9DE270}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{8A7E05DF-A544-4D43-B47E-603BCF60EA21}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-21140" windowWidth="38400" windowHeight="21140" activeTab="1" xr2:uid="{6937E72E-728A-D145-8CDA-D71DF27F887B}"/>
+    <workbookView xWindow="-100" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="1" xr2:uid="{6937E72E-728A-D145-8CDA-D71DF27F887B}"/>
   </bookViews>
   <sheets>
     <sheet name="Current expenditure" sheetId="1" r:id="rId1"/>
@@ -818,7 +818,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1057,8 +1057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60C6C199-5511-6948-BFE1-269E2A0DC50C}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1101,9 +1101,7 @@
         <f>(20+30+45+45+35+22)/6 * 1000000</f>
         <v>32833333.333333336</v>
       </c>
-      <c r="E2" s="11" t="s">
-        <v>20</v>
-      </c>
+      <c r="E2" s="11"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
@@ -1134,7 +1132,9 @@
         <f>(20+30+45+45+35+22)/6 * 1000000</f>
         <v>32833333.333333336</v>
       </c>
-      <c r="E4" s="11"/>
+      <c r="E4" s="11" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">

</xml_diff>